<commit_message>
4G y 5G OK
</commit_message>
<xml_diff>
--- a/Macro_4G_Streamlit/LA781 - TEKNICA/LA781 - TEKNICA/WSHReport.xlsx
+++ b/Macro_4G_Streamlit/LA781 - TEKNICA/LA781 - TEKNICA/WSHReport.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olitelltda-my.sharepoint.com/personal/jcavieres_olitel_cl/Documents/000_Shared_Integracion/2025/RAN/011-Noviembre/LA781 - TEKNICA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pledesma\Documents\Piero Ledesma\Piero Ledesma\Nuevas Macros\Macro_4G_Streamlit\LA781 - TEKNICA\LA781 - TEKNICA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="835" documentId="11_28FC42E91A06E4CB3C6A2339DCF99A4544BD8687" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D2D6298-4746-4534-99B9-BD40D715B907}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="1140" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2G-3G" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="RANSHARING_WOM" sheetId="4" r:id="rId4"/>
     <sheet name="CLuster 5G" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="229">
   <si>
     <t>Nemonico</t>
   </si>
@@ -722,17 +721,33 @@
   </si>
   <si>
     <t>VLAN_4G_TRAFFIC_MIMO</t>
+  </si>
+  <si>
+    <t>GLA781</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -761,9 +776,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,7 +1084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AU3"/>
   <sheetViews>
@@ -1426,12 +1443,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,8 +1579,8 @@
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>97</v>
+      <c r="A2" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1630,7 +1647,7 @@
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B3" t="s">
@@ -1707,12 +1724,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,7 +2185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:W1"/>
   <sheetViews>
@@ -2254,7 +2271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:CJ1"/>
   <sheetViews>

</xml_diff>